<commit_message>
Line count update For this branch (not Main)
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotoClubHubLinecount.xlsx
+++ b/Fotogroep Waalre/Documentation/FotoClubHubLinecount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A5DC47-F34F-184C-AA50-228298976C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E7A970-17B7-5A42-8EE4-EED7B0D79FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -800,6 +800,9 @@
                 <c:pt idx="178">
                   <c:v>45184</c:v>
                 </c:pt>
+                <c:pt idx="179">
+                  <c:v>45186</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1345,6 +1348,9 @@
                 </c:pt>
                 <c:pt idx="178">
                   <c:v>5180</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>5205</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1929,6 +1935,9 @@
                 <c:pt idx="178">
                   <c:v>45184</c:v>
                 </c:pt>
+                <c:pt idx="179">
+                  <c:v>45186</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2474,6 +2483,9 @@
                 </c:pt>
                 <c:pt idx="178">
                   <c:v>4107</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>4126</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3060,6 +3072,9 @@
                 <c:pt idx="178">
                   <c:v>45184</c:v>
                 </c:pt>
+                <c:pt idx="179">
+                  <c:v>45186</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3605,6 +3620,9 @@
                 </c:pt>
                 <c:pt idx="178">
                   <c:v>589</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>594</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4210,6 +4228,9 @@
                 <c:pt idx="178">
                   <c:v>45184</c:v>
                 </c:pt>
+                <c:pt idx="179">
+                  <c:v>45186</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4755,6 +4776,9 @@
                 </c:pt>
                 <c:pt idx="178">
                   <c:v>484</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>485</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5983,13 +6007,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K181"/>
+  <dimension ref="A1:K182"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B125" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I182" sqref="I182"/>
+      <selection pane="bottomRight" activeCell="I183" sqref="I183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12708,6 +12732,43 @@
       </c>
       <c r="K181" s="7">
         <v>484</v>
+      </c>
+    </row>
+    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A182" s="1">
+        <v>45186</v>
+      </c>
+      <c r="B182" s="2">
+        <v>9</v>
+      </c>
+      <c r="C182">
+        <f t="shared" ref="C182" si="280">SUM(D182:F182)</f>
+        <v>1673</v>
+      </c>
+      <c r="D182">
+        <v>1105</v>
+      </c>
+      <c r="E182">
+        <v>371</v>
+      </c>
+      <c r="F182" s="3">
+        <v>197</v>
+      </c>
+      <c r="G182" s="4">
+        <v>58</v>
+      </c>
+      <c r="H182">
+        <f t="shared" ref="H182" si="281">SUM(I182:K182)</f>
+        <v>5205</v>
+      </c>
+      <c r="I182" s="5">
+        <v>4126</v>
+      </c>
+      <c r="J182" s="6">
+        <v>594</v>
+      </c>
+      <c r="K182" s="7">
+        <v>485</v>
       </c>
     </row>
   </sheetData>
@@ -12727,7 +12788,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AA42" sqref="AA42"/>
     </sheetView>
   </sheetViews>

</xml_diff>